<commit_message>
GDE-6408 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ08_ComprehensiveDeal.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ08_ComprehensiveDeal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="10" activeTab="14" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="13" activeTab="16" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -133,12 +133,6 @@
       <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-      <color indexed="81"/>
-      <sz val="9"/>
     </font>
   </fonts>
   <fills count="12">
@@ -297,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -453,57 +447,19 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>tc={18C058B7-AD06-4252-A501-0281D3A8D732}</author>
-    <author>tc={AEC386EB-7EFE-46CB-9039-917A25DD9A33}</author>
-    <author>tc={8CF56A1B-6622-447E-B66C-D7E348EFC810}</author>
-    <author>tc={EC7B3D7C-A3BF-4A03-AAB9-CEDA9DEAE88D}</author>
-  </authors>
-  <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    For Lender1</t>
-      </text>
-    </comment>
-    <comment ref="AA1" authorId="1" shapeId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    For Lender1</t>
-      </text>
-    </comment>
-    <comment ref="AB1" authorId="2" shapeId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    For Lender2</t>
-      </text>
-    </comment>
-    <comment ref="AC1" authorId="3" shapeId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    For Lender2</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2758,8 +2714,8 @@
   </sheetPr>
   <dimension ref="A1:AU4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU7" sqref="AU7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2846,7 +2802,7 @@
           <t>Borrower_ShortName</t>
         </is>
       </c>
-      <c r="I1" s="79" t="inlineStr">
+      <c r="I1" s="77" t="inlineStr">
         <is>
           <t>Calendar</t>
         </is>
@@ -2856,7 +2812,7 @@
           <t>Loan_PricingOption</t>
         </is>
       </c>
-      <c r="K1" s="25" t="inlineStr">
+      <c r="K1" s="77" t="inlineStr">
         <is>
           <t>Facility_Currency</t>
         </is>
@@ -3063,7 +3019,7 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="G2" s="89" t="inlineStr">
         <is>
           <t>S8TERM14092020165659</t>
         </is>
@@ -3073,7 +3029,7 @@
           <t>CUSTSHORT59122</t>
         </is>
       </c>
-      <c r="I2" s="36" t="inlineStr">
+      <c r="I2" s="86" t="inlineStr">
         <is>
           <t>Sydney, Australia</t>
         </is>
@@ -3083,7 +3039,7 @@
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="K2" s="36" t="inlineStr">
+      <c r="K2" s="86" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
@@ -3098,12 +3054,12 @@
           <t>20,000,000.00</t>
         </is>
       </c>
-      <c r="N2" s="27" t="inlineStr">
+      <c r="N2" s="88" t="inlineStr">
         <is>
           <t>16-Oct-2018</t>
         </is>
       </c>
-      <c r="O2" s="27" t="inlineStr">
+      <c r="O2" s="88" t="inlineStr">
         <is>
           <t>18-Apr-2020</t>
         </is>
@@ -3185,7 +3141,7 @@
       <c r="AF2" s="75" t="n">
         <v>20</v>
       </c>
-      <c r="AG2" s="75" t="inlineStr">
+      <c r="AG2" s="87" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/012689</t>
         </is>
@@ -3235,7 +3191,7 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="AQ2" s="75" t="n"/>
+      <c r="AQ2" s="87" t="n"/>
       <c r="AR2" s="3" t="inlineStr">
         <is>
           <t>27,000,000.00</t>
@@ -3280,7 +3236,7 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="G3" s="89" t="inlineStr">
         <is>
           <t>S8TERM14092020165659</t>
         </is>
@@ -3290,12 +3246,13 @@
           <t>CUSTSHORT59122</t>
         </is>
       </c>
+      <c r="I3" s="86" t="n"/>
       <c r="J3" s="36" t="inlineStr">
         <is>
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="K3" s="36" t="inlineStr">
+      <c r="K3" s="86" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
@@ -3310,12 +3267,12 @@
           <t>7,000,000.00</t>
         </is>
       </c>
-      <c r="N3" s="27" t="inlineStr">
+      <c r="N3" s="88" t="inlineStr">
         <is>
           <t>16-Oct-2018</t>
         </is>
       </c>
-      <c r="O3" s="27" t="inlineStr">
+      <c r="O3" s="88" t="inlineStr">
         <is>
           <t>18-Apr-2020</t>
         </is>
@@ -3343,17 +3300,17 @@
           <t>Base Rate changed to 2.25%</t>
         </is>
       </c>
-      <c r="U3" s="36" t="inlineStr">
+      <c r="U3" s="86" t="inlineStr">
         <is>
           <t>CUSTSHORT59122</t>
         </is>
       </c>
-      <c r="V3" s="36" t="inlineStr">
+      <c r="V3" s="86" t="inlineStr">
         <is>
           <t>BDOLEND44119</t>
         </is>
       </c>
-      <c r="W3" s="36" t="inlineStr">
+      <c r="W3" s="86" t="inlineStr">
         <is>
           <t>BPILEND28140</t>
         </is>
@@ -3397,7 +3354,7 @@
       <c r="AF3" s="75" t="n">
         <v>20</v>
       </c>
-      <c r="AG3" s="75" t="inlineStr">
+      <c r="AG3" s="87" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/012689</t>
         </is>
@@ -3447,7 +3404,7 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="AQ3" s="75" t="n"/>
+      <c r="AQ3" s="87" t="n"/>
     </row>
     <row r="4" customFormat="1" s="36">
       <c r="A4" s="36" t="inlineStr">
@@ -3472,7 +3429,7 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>60000324</t>
+          <t>60000011</t>
         </is>
       </c>
       <c r="F4" s="36" t="inlineStr">
@@ -3480,7 +3437,7 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="G4" s="89" t="inlineStr">
         <is>
           <t>S8TERM14092020165659</t>
         </is>
@@ -3490,12 +3447,13 @@
           <t>CUSTSHORT59122</t>
         </is>
       </c>
+      <c r="I4" s="86" t="n"/>
       <c r="J4" s="75" t="inlineStr">
         <is>
           <t>USD LIBOR Option</t>
         </is>
       </c>
-      <c r="K4" s="75" t="n"/>
+      <c r="K4" s="87" t="n"/>
       <c r="L4" s="36" t="inlineStr">
         <is>
           <t>USD</t>
@@ -3506,6 +3464,8 @@
           <t>15,000,000.00</t>
         </is>
       </c>
+      <c r="N4" s="86" t="n"/>
+      <c r="O4" s="86" t="n"/>
       <c r="P4" s="81" t="n">
         <v>41389</v>
       </c>
@@ -3514,39 +3474,58 @@
           <t>2 Days</t>
         </is>
       </c>
+      <c r="R4" s="86" t="n"/>
       <c r="S4" s="36" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
+      <c r="T4" s="86" t="n"/>
+      <c r="U4" s="86" t="n"/>
+      <c r="V4" s="86" t="n"/>
+      <c r="W4" s="86" t="n"/>
       <c r="X4" s="36" t="inlineStr">
         <is>
-          <t>IMT</t>
+          <t>DDA</t>
         </is>
       </c>
       <c r="Y4" s="36" t="inlineStr">
         <is>
-          <t>IMTUSD1-0522</t>
+          <t>DDA3</t>
         </is>
       </c>
       <c r="Z4" s="36" t="inlineStr">
         <is>
-          <t>RTGS</t>
+          <t>DDA</t>
         </is>
       </c>
       <c r="AA4" s="36" t="inlineStr">
         <is>
-          <t>RTGS1</t>
+          <t>DDA2</t>
         </is>
       </c>
       <c r="AB4" s="36" t="inlineStr">
         <is>
-          <t>RTGS</t>
+          <t>DDA</t>
         </is>
       </c>
       <c r="AC4" s="36" t="inlineStr">
         <is>
-          <t>RTGS1</t>
+          <t>DDA2</t>
+        </is>
+      </c>
+      <c r="AD4" s="75" t="n">
+        <v>55</v>
+      </c>
+      <c r="AE4" s="75" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF4" s="75" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG4" s="87" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/012689</t>
         </is>
       </c>
       <c r="AH4" s="42" t="inlineStr">
@@ -3604,7 +3583,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" pageOrder="overThenDown" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -3716,10 +3694,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3788,12 +3766,12 @@
           <t>TransactionNo_Prefix</t>
         </is>
       </c>
-      <c r="G1" s="39" t="inlineStr">
+      <c r="G1" s="91" t="inlineStr">
         <is>
           <t>PricingChange_TransactionNo</t>
         </is>
       </c>
-      <c r="H1" s="39" t="inlineStr">
+      <c r="H1" s="91" t="inlineStr">
         <is>
           <t>PricingChange_EffectiveDate</t>
         </is>
@@ -3957,12 +3935,12 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>TRN4304</t>
+          <t>TRN1515</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>05-Mar-2019</t>
+          <t>24-Apr-2013</t>
         </is>
       </c>
       <c r="I2" s="75" t="inlineStr">
@@ -4070,6 +4048,13 @@
           <t>Awaiting Release</t>
         </is>
       </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="90" t="n"/>
+      <c r="D3" s="90" t="n"/>
+      <c r="E3" s="90" t="n"/>
+      <c r="F3" s="90" t="n"/>
+      <c r="I3" s="90" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -4287,7 +4272,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>60000324</t>
+          <t>60000011</t>
         </is>
       </c>
       <c r="J2" s="27" t="inlineStr">
@@ -7103,7 +7088,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="C4" s="44" t="n"/>
       <c r="T4" s="75" t="inlineStr">
@@ -7263,16 +7247,10 @@
       <c r="AK6" s="31" t="n"/>
       <c r="AL6" s="31" t="n"/>
     </row>
-    <row r="7"/>
     <row r="8">
       <c r="R8" s="75" t="n"/>
       <c r="U8" s="30" t="n"/>
     </row>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
     <row r="14">
       <c r="C14" s="36" t="n"/>
       <c r="E14" s="36" t="n"/>

</xml_diff>

<commit_message>
GDE-6409 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ08_ComprehensiveDeal.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ08_ComprehensiveDeal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="10" activeTab="14" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="15" activeTab="18" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -133,12 +133,6 @@
       <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-      <color indexed="81"/>
-      <sz val="9"/>
     </font>
   </fonts>
   <fills count="12">
@@ -297,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -453,57 +447,22 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>tc={18C058B7-AD06-4252-A501-0281D3A8D732}</author>
-    <author>tc={AEC386EB-7EFE-46CB-9039-917A25DD9A33}</author>
-    <author>tc={8CF56A1B-6622-447E-B66C-D7E348EFC810}</author>
-    <author>tc={EC7B3D7C-A3BF-4A03-AAB9-CEDA9DEAE88D}</author>
-  </authors>
-  <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    For Lender1</t>
-      </text>
-    </comment>
-    <comment ref="AA1" authorId="1" shapeId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    For Lender1</t>
-      </text>
-    </comment>
-    <comment ref="AB1" authorId="2" shapeId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    For Lender2</t>
-      </text>
-    </comment>
-    <comment ref="AC1" authorId="3" shapeId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    For Lender2</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2758,8 +2717,8 @@
   </sheetPr>
   <dimension ref="A1:AU4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU7" sqref="AU7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2846,7 +2805,7 @@
           <t>Borrower_ShortName</t>
         </is>
       </c>
-      <c r="I1" s="79" t="inlineStr">
+      <c r="I1" s="77" t="inlineStr">
         <is>
           <t>Calendar</t>
         </is>
@@ -2856,7 +2815,7 @@
           <t>Loan_PricingOption</t>
         </is>
       </c>
-      <c r="K1" s="25" t="inlineStr">
+      <c r="K1" s="77" t="inlineStr">
         <is>
           <t>Facility_Currency</t>
         </is>
@@ -3063,7 +3022,7 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="G2" s="89" t="inlineStr">
         <is>
           <t>S8TERM14092020165659</t>
         </is>
@@ -3073,7 +3032,7 @@
           <t>CUSTSHORT59122</t>
         </is>
       </c>
-      <c r="I2" s="36" t="inlineStr">
+      <c r="I2" s="86" t="inlineStr">
         <is>
           <t>Sydney, Australia</t>
         </is>
@@ -3083,7 +3042,7 @@
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="K2" s="36" t="inlineStr">
+      <c r="K2" s="86" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
@@ -3098,12 +3057,12 @@
           <t>20,000,000.00</t>
         </is>
       </c>
-      <c r="N2" s="27" t="inlineStr">
+      <c r="N2" s="88" t="inlineStr">
         <is>
           <t>16-Oct-2018</t>
         </is>
       </c>
-      <c r="O2" s="27" t="inlineStr">
+      <c r="O2" s="88" t="inlineStr">
         <is>
           <t>18-Apr-2020</t>
         </is>
@@ -3185,7 +3144,7 @@
       <c r="AF2" s="75" t="n">
         <v>20</v>
       </c>
-      <c r="AG2" s="75" t="inlineStr">
+      <c r="AG2" s="87" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/012689</t>
         </is>
@@ -3235,7 +3194,7 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="AQ2" s="75" t="n"/>
+      <c r="AQ2" s="87" t="n"/>
       <c r="AR2" s="3" t="inlineStr">
         <is>
           <t>27,000,000.00</t>
@@ -3280,7 +3239,7 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="G3" s="89" t="inlineStr">
         <is>
           <t>S8TERM14092020165659</t>
         </is>
@@ -3290,12 +3249,13 @@
           <t>CUSTSHORT59122</t>
         </is>
       </c>
+      <c r="I3" s="86" t="n"/>
       <c r="J3" s="36" t="inlineStr">
         <is>
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="K3" s="36" t="inlineStr">
+      <c r="K3" s="86" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
@@ -3310,12 +3270,12 @@
           <t>7,000,000.00</t>
         </is>
       </c>
-      <c r="N3" s="27" t="inlineStr">
+      <c r="N3" s="88" t="inlineStr">
         <is>
           <t>16-Oct-2018</t>
         </is>
       </c>
-      <c r="O3" s="27" t="inlineStr">
+      <c r="O3" s="88" t="inlineStr">
         <is>
           <t>18-Apr-2020</t>
         </is>
@@ -3343,17 +3303,17 @@
           <t>Base Rate changed to 2.25%</t>
         </is>
       </c>
-      <c r="U3" s="36" t="inlineStr">
+      <c r="U3" s="86" t="inlineStr">
         <is>
           <t>CUSTSHORT59122</t>
         </is>
       </c>
-      <c r="V3" s="36" t="inlineStr">
+      <c r="V3" s="86" t="inlineStr">
         <is>
           <t>BDOLEND44119</t>
         </is>
       </c>
-      <c r="W3" s="36" t="inlineStr">
+      <c r="W3" s="86" t="inlineStr">
         <is>
           <t>BPILEND28140</t>
         </is>
@@ -3397,7 +3357,7 @@
       <c r="AF3" s="75" t="n">
         <v>20</v>
       </c>
-      <c r="AG3" s="75" t="inlineStr">
+      <c r="AG3" s="87" t="inlineStr">
         <is>
           <t>CB001/Hold for Investment - Australia/012689</t>
         </is>
@@ -3447,7 +3407,7 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="AQ3" s="75" t="n"/>
+      <c r="AQ3" s="87" t="n"/>
     </row>
     <row r="4" customFormat="1" s="36">
       <c r="A4" s="36" t="inlineStr">
@@ -3472,7 +3432,7 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>60000324</t>
+          <t>60000011</t>
         </is>
       </c>
       <c r="F4" s="36" t="inlineStr">
@@ -3480,7 +3440,7 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="G4" s="89" t="inlineStr">
         <is>
           <t>S8TERM14092020165659</t>
         </is>
@@ -3490,12 +3450,13 @@
           <t>CUSTSHORT59122</t>
         </is>
       </c>
+      <c r="I4" s="86" t="n"/>
       <c r="J4" s="75" t="inlineStr">
         <is>
           <t>USD LIBOR Option</t>
         </is>
       </c>
-      <c r="K4" s="75" t="n"/>
+      <c r="K4" s="87" t="n"/>
       <c r="L4" s="36" t="inlineStr">
         <is>
           <t>USD</t>
@@ -3506,6 +3467,8 @@
           <t>15,000,000.00</t>
         </is>
       </c>
+      <c r="N4" s="86" t="n"/>
+      <c r="O4" s="86" t="n"/>
       <c r="P4" s="81" t="n">
         <v>41389</v>
       </c>
@@ -3514,39 +3477,58 @@
           <t>2 Days</t>
         </is>
       </c>
+      <c r="R4" s="86" t="n"/>
       <c r="S4" s="36" t="inlineStr">
         <is>
           <t>to the actual due date</t>
         </is>
       </c>
+      <c r="T4" s="86" t="n"/>
+      <c r="U4" s="86" t="n"/>
+      <c r="V4" s="86" t="n"/>
+      <c r="W4" s="86" t="n"/>
       <c r="X4" s="36" t="inlineStr">
         <is>
-          <t>IMT</t>
+          <t>DDA</t>
         </is>
       </c>
       <c r="Y4" s="36" t="inlineStr">
         <is>
-          <t>IMTUSD1-0522</t>
+          <t>DDA3</t>
         </is>
       </c>
       <c r="Z4" s="36" t="inlineStr">
         <is>
-          <t>RTGS</t>
+          <t>DDA</t>
         </is>
       </c>
       <c r="AA4" s="36" t="inlineStr">
         <is>
-          <t>RTGS1</t>
+          <t>DDA2</t>
         </is>
       </c>
       <c r="AB4" s="36" t="inlineStr">
         <is>
-          <t>RTGS</t>
+          <t>DDA</t>
         </is>
       </c>
       <c r="AC4" s="36" t="inlineStr">
         <is>
-          <t>RTGS1</t>
+          <t>DDA2</t>
+        </is>
+      </c>
+      <c r="AD4" s="75" t="n">
+        <v>55</v>
+      </c>
+      <c r="AE4" s="75" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF4" s="75" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG4" s="87" t="inlineStr">
+        <is>
+          <t>CB001/Hold for Investment - Australia/012689</t>
         </is>
       </c>
       <c r="AH4" s="42" t="inlineStr">
@@ -3604,7 +3586,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" pageOrder="overThenDown" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
@@ -3716,10 +3697,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3788,12 +3769,12 @@
           <t>TransactionNo_Prefix</t>
         </is>
       </c>
-      <c r="G1" s="39" t="inlineStr">
+      <c r="G1" s="91" t="inlineStr">
         <is>
           <t>PricingChange_TransactionNo</t>
         </is>
       </c>
-      <c r="H1" s="39" t="inlineStr">
+      <c r="H1" s="91" t="inlineStr">
         <is>
           <t>PricingChange_EffectiveDate</t>
         </is>
@@ -3957,12 +3938,12 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>TRN4304</t>
+          <t>TRN1515</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>05-Mar-2019</t>
+          <t>24-Apr-2013</t>
         </is>
       </c>
       <c r="I2" s="75" t="inlineStr">
@@ -4070,6 +4051,13 @@
           <t>Awaiting Release</t>
         </is>
       </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="90" t="n"/>
+      <c r="D3" s="90" t="n"/>
+      <c r="E3" s="90" t="n"/>
+      <c r="F3" s="90" t="n"/>
+      <c r="I3" s="90" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -4084,10 +4072,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4097,12 +4085,14 @@
     <col width="22.5703125" customWidth="1" style="27" min="3" max="3"/>
     <col width="20.140625" customWidth="1" style="27" min="4" max="4"/>
     <col width="21.5703125" customWidth="1" style="27" min="5" max="5"/>
-    <col width="18.42578125" customWidth="1" style="27" min="6" max="6"/>
+    <col width="9.140625" bestFit="1" customWidth="1" style="27" min="6" max="6"/>
     <col width="12.7109375" customWidth="1" style="27" min="7" max="8"/>
     <col width="18.7109375" customWidth="1" style="27" min="9" max="9"/>
     <col width="24.28515625" customWidth="1" style="27" min="10" max="10"/>
     <col width="12.42578125" customWidth="1" style="27" min="11" max="11"/>
-    <col width="18.7109375" customWidth="1" style="75" min="12" max="14"/>
+    <col width="17.85546875" bestFit="1" customWidth="1" style="75" min="12" max="12"/>
+    <col width="18.7109375" customWidth="1" style="75" min="13" max="13"/>
+    <col width="13.42578125" bestFit="1" customWidth="1" style="75" min="14" max="14"/>
     <col width="17.7109375" customWidth="1" style="75" min="15" max="15"/>
     <col width="9" customWidth="1" style="27" min="16" max="16"/>
     <col width="17.42578125" customWidth="1" style="27" min="17" max="17"/>
@@ -4114,7 +4104,13 @@
     <col width="9" customWidth="1" style="27" min="24" max="25"/>
     <col width="8" customWidth="1" style="27" min="26" max="26"/>
     <col width="16" customWidth="1" style="36" min="27" max="27"/>
-    <col width="14.28515625" bestFit="1" customWidth="1" min="28" max="28"/>
+    <col width="17.42578125" bestFit="1" customWidth="1" min="28" max="28"/>
+    <col width="19.85546875" bestFit="1" customWidth="1" min="29" max="29"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" min="30" max="31"/>
+    <col width="26.5703125" bestFit="1" customWidth="1" min="32" max="32"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" min="33" max="34"/>
+    <col width="21.140625" bestFit="1" customWidth="1" min="35" max="35"/>
+    <col width="20.140625" bestFit="1" customWidth="1" min="36" max="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="26">
@@ -4148,17 +4144,17 @@
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="G1" s="26" t="inlineStr">
+      <c r="G1" s="94" t="inlineStr">
         <is>
           <t>Repricing_Type</t>
         </is>
       </c>
-      <c r="H1" s="26" t="inlineStr">
+      <c r="H1" s="94" t="inlineStr">
         <is>
           <t>Repricing_Date</t>
         </is>
       </c>
-      <c r="I1" s="26" t="inlineStr">
+      <c r="I1" s="94" t="inlineStr">
         <is>
           <t>Repricing_Add_Option</t>
         </is>
@@ -4168,32 +4164,32 @@
           <t>Repricing_Add_Option_Setup</t>
         </is>
       </c>
-      <c r="K1" s="26" t="inlineStr">
+      <c r="K1" s="94" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
       </c>
-      <c r="L1" s="25" t="inlineStr">
+      <c r="L1" s="79" t="inlineStr">
         <is>
           <t>Contact_Email</t>
         </is>
       </c>
-      <c r="M1" s="25" t="inlineStr">
+      <c r="M1" s="79" t="inlineStr">
         <is>
           <t>Notice_ContactPerson</t>
         </is>
       </c>
-      <c r="N1" s="25" t="inlineStr">
+      <c r="N1" s="79" t="inlineStr">
         <is>
           <t>Notice_Method</t>
         </is>
       </c>
-      <c r="O1" s="25" t="inlineStr">
+      <c r="O1" s="79" t="inlineStr">
         <is>
           <t>Lender1_ShortName</t>
         </is>
       </c>
-      <c r="P1" s="26" t="inlineStr">
+      <c r="P1" s="94" t="inlineStr">
         <is>
           <t>Base_Rate</t>
         </is>
@@ -4256,6 +4252,51 @@
       <c r="AB1" s="26" t="inlineStr">
         <is>
           <t>Borrower_Name</t>
+        </is>
+      </c>
+      <c r="AC1" s="25" t="inlineStr">
+        <is>
+          <t>BorrowerContact_Email</t>
+        </is>
+      </c>
+      <c r="AD1" s="25" t="inlineStr">
+        <is>
+          <t>Lender1Contact_Email</t>
+        </is>
+      </c>
+      <c r="AE1" s="25" t="inlineStr">
+        <is>
+          <t>Lender2Contact_Email</t>
+        </is>
+      </c>
+      <c r="AF1" s="25" t="inlineStr">
+        <is>
+          <t>Notice_BorrowerContactPerson</t>
+        </is>
+      </c>
+      <c r="AG1" s="25" t="inlineStr">
+        <is>
+          <t>Notice_Lender1ContactPerson</t>
+        </is>
+      </c>
+      <c r="AH1" s="25" t="inlineStr">
+        <is>
+          <t>Notice_Lender2ContactPerson</t>
+        </is>
+      </c>
+      <c r="AI1" s="25" t="inlineStr">
+        <is>
+          <t>Notice_BorrowerMethod</t>
+        </is>
+      </c>
+      <c r="AJ1" s="25" t="inlineStr">
+        <is>
+          <t>Notice_Lender1Method</t>
+        </is>
+      </c>
+      <c r="AK1" s="25" t="inlineStr">
+        <is>
+          <t>Notice_Lender2Method</t>
         </is>
       </c>
     </row>
@@ -4287,7 +4328,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>60000324</t>
+          <t>60000011</t>
         </is>
       </c>
       <c r="J2" s="27" t="inlineStr">
@@ -4385,16 +4426,74 @@
           <t>CUSTSHORT59122</t>
         </is>
       </c>
-      <c r="AC2" s="3" t="n"/>
-      <c r="AD2" s="3" t="n"/>
-      <c r="AE2" s="3" t="n"/>
-      <c r="AF2" s="3" t="n"/>
-      <c r="AG2" s="3" t="n"/>
-      <c r="AH2" s="3" t="n"/>
-      <c r="AI2" s="3" t="n"/>
-      <c r="AJ2" s="3" t="n"/>
-      <c r="AK2" s="3" t="n"/>
+      <c r="AC2" s="42" t="inlineStr">
+        <is>
+          <t>john.blogg@abc.com</t>
+        </is>
+      </c>
+      <c r="AD2" s="36" t="inlineStr">
+        <is>
+          <t>darlonhijara@abc.com</t>
+        </is>
+      </c>
+      <c r="AE2" s="36" t="inlineStr">
+        <is>
+          <t>darlonhijara@abc.com</t>
+        </is>
+      </c>
+      <c r="AF2" s="75" t="inlineStr">
+        <is>
+          <t>John Bloggs</t>
+        </is>
+      </c>
+      <c r="AG2" s="75" t="inlineStr">
+        <is>
+          <t>Darlon Hijara</t>
+        </is>
+      </c>
+      <c r="AH2" s="75" t="inlineStr">
+        <is>
+          <t>DarlonJeremiah Hijaratwo</t>
+        </is>
+      </c>
+      <c r="AI2" s="75" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="AJ2" s="75" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="AK2" s="75" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
       <c r="AL2" s="3" t="n"/>
+    </row>
+    <row r="3">
+      <c r="D3" s="92" t="n"/>
+      <c r="E3" s="92" t="n"/>
+      <c r="F3" s="92" t="n"/>
+      <c r="J3" s="92" t="n"/>
+      <c r="Q3" s="92" t="n"/>
+      <c r="T3" s="92" t="n"/>
+      <c r="V3" s="92" t="n"/>
+      <c r="W3" s="92" t="n"/>
+      <c r="X3" s="92" t="n"/>
+      <c r="Y3" s="92" t="n"/>
+      <c r="Z3" s="92" t="n"/>
+      <c r="AC3" s="93" t="n"/>
+      <c r="AD3" s="93" t="n"/>
+      <c r="AE3" s="93" t="n"/>
+      <c r="AF3" s="93" t="n"/>
+      <c r="AG3" s="93" t="n"/>
+      <c r="AH3" s="93" t="n"/>
+      <c r="AI3" s="93" t="n"/>
+      <c r="AJ3" s="93" t="n"/>
+      <c r="AK3" s="93" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -4409,10 +4508,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4480,172 +4579,172 @@
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="E1" s="39" t="inlineStr">
+      <c r="E1" s="91" t="inlineStr">
         <is>
           <t>Current_Cmt</t>
         </is>
       </c>
-      <c r="F1" s="39" t="inlineStr">
+      <c r="F1" s="91" t="inlineStr">
         <is>
           <t>Contr_Gross</t>
         </is>
       </c>
-      <c r="G1" s="39" t="inlineStr">
+      <c r="G1" s="91" t="inlineStr">
         <is>
           <t>Net_Cmt</t>
         </is>
       </c>
-      <c r="H1" s="39" t="inlineStr">
+      <c r="H1" s="74" t="inlineStr">
         <is>
           <t>HostBank_Lender</t>
         </is>
       </c>
-      <c r="I1" s="39" t="inlineStr">
+      <c r="I1" s="74" t="inlineStr">
         <is>
           <t>Lender1</t>
         </is>
       </c>
-      <c r="J1" s="39" t="inlineStr">
+      <c r="J1" s="74" t="inlineStr">
         <is>
           <t>Lender2</t>
         </is>
       </c>
-      <c r="K1" s="39" t="inlineStr">
+      <c r="K1" s="91" t="inlineStr">
         <is>
           <t>Original_UIHBActualAmount</t>
         </is>
       </c>
-      <c r="L1" s="39" t="inlineStr">
+      <c r="L1" s="91" t="inlineStr">
         <is>
           <t>Original_UILender1ActualAmount</t>
         </is>
       </c>
-      <c r="M1" s="39" t="inlineStr">
+      <c r="M1" s="91" t="inlineStr">
         <is>
           <t>Original_UILender2ActualAmount</t>
         </is>
       </c>
-      <c r="N1" s="39" t="inlineStr">
+      <c r="N1" s="91" t="inlineStr">
         <is>
           <t>Orig_PrimariesAssignees_ActualTotal</t>
         </is>
       </c>
-      <c r="O1" s="39" t="inlineStr">
+      <c r="O1" s="91" t="inlineStr">
         <is>
           <t>Original_UIHBSharesActualAmount</t>
         </is>
       </c>
-      <c r="P1" s="39" t="inlineStr">
+      <c r="P1" s="91" t="inlineStr">
         <is>
           <t>Orig_HostBankShares_ActualNetAllTotal</t>
         </is>
       </c>
-      <c r="Q1" s="39" t="inlineStr">
+      <c r="Q1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityCurrentCmt</t>
         </is>
       </c>
-      <c r="R1" s="39" t="inlineStr">
+      <c r="R1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityAvailableToDraw</t>
         </is>
       </c>
-      <c r="S1" s="39" t="inlineStr">
+      <c r="S1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityHBContrGross</t>
         </is>
       </c>
-      <c r="T1" s="39" t="inlineStr">
+      <c r="T1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityHBOutstandings</t>
         </is>
       </c>
-      <c r="U1" s="39" t="inlineStr">
+      <c r="U1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityHBAvailToDraw</t>
         </is>
       </c>
-      <c r="V1" s="39" t="inlineStr">
+      <c r="V1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityNetCmt</t>
         </is>
       </c>
-      <c r="W1" s="39" t="inlineStr">
+      <c r="W1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityHBNetFundableCmt</t>
         </is>
       </c>
-      <c r="X1" s="39" t="inlineStr">
+      <c r="X1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityHBNetOutstandings_Funded</t>
         </is>
       </c>
-      <c r="Y1" s="39" t="inlineStr">
+      <c r="Y1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityHBNetAvailToDraw_Fundable</t>
         </is>
       </c>
-      <c r="Z1" s="39" t="inlineStr">
+      <c r="Z1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacilityHBNetAvailToDraw</t>
         </is>
       </c>
-      <c r="AA1" s="39" t="inlineStr">
+      <c r="AA1" s="91" t="inlineStr">
         <is>
           <t>Original_UIFacHBActualAmount</t>
         </is>
       </c>
-      <c r="AB1" s="39" t="inlineStr">
+      <c r="AB1" s="91" t="inlineStr">
         <is>
           <t>Original_UIFacLender1ActualAmount</t>
         </is>
       </c>
-      <c r="AC1" s="39" t="inlineStr">
+      <c r="AC1" s="91" t="inlineStr">
         <is>
           <t>Original_UIFacLender2ActualAmount</t>
         </is>
       </c>
-      <c r="AD1" s="39" t="inlineStr">
+      <c r="AD1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacPrimariesAssignees_ActualTotal</t>
         </is>
       </c>
-      <c r="AE1" s="39" t="inlineStr">
+      <c r="AE1" s="91" t="inlineStr">
         <is>
           <t>Original_UIFacHBSharesActualAmount</t>
         </is>
       </c>
-      <c r="AF1" s="39" t="inlineStr">
+      <c r="AF1" s="91" t="inlineStr">
         <is>
           <t>Orig_FacHostBankShares_ActualNetAllTotal</t>
         </is>
       </c>
-      <c r="AG1" s="39" t="inlineStr">
+      <c r="AG1" s="91" t="inlineStr">
         <is>
           <t>Computed_HBActualAmount</t>
         </is>
       </c>
-      <c r="AH1" s="39" t="inlineStr">
+      <c r="AH1" s="91" t="inlineStr">
         <is>
           <t>Computed_Lender1ActualAmount</t>
         </is>
       </c>
-      <c r="AI1" s="39" t="inlineStr">
+      <c r="AI1" s="91" t="inlineStr">
         <is>
           <t>Computed_Lender2ActualAmount</t>
         </is>
       </c>
-      <c r="AJ1" s="39" t="inlineStr">
+      <c r="AJ1" s="91" t="inlineStr">
         <is>
           <t>HBShares_UIActualAmount</t>
         </is>
       </c>
-      <c r="AK1" s="39" t="inlineStr">
+      <c r="AK1" s="91" t="inlineStr">
         <is>
           <t>Updated_UIFaciltyCurrentCmt</t>
         </is>
       </c>
-      <c r="AL1" s="39" t="inlineStr">
+      <c r="AL1" s="91" t="inlineStr">
         <is>
           <t>AMD_EffectiveDate</t>
         </is>
@@ -4655,7 +4754,7 @@
           <t>AmendmentNumber_Prefix</t>
         </is>
       </c>
-      <c r="AN1" s="39" t="inlineStr">
+      <c r="AN1" s="91" t="inlineStr">
         <is>
           <t>AmendmentNo</t>
         </is>
@@ -4680,17 +4779,17 @@
           <t>AmortSched_Status</t>
         </is>
       </c>
-      <c r="AS1" s="39" t="inlineStr">
+      <c r="AS1" s="74" t="inlineStr">
         <is>
           <t>HostBankLender_Percentage</t>
         </is>
       </c>
-      <c r="AT1" s="39" t="inlineStr">
+      <c r="AT1" s="74" t="inlineStr">
         <is>
           <t>Lender1_Percentage</t>
         </is>
       </c>
-      <c r="AU1" s="39" t="inlineStr">
+      <c r="AU1" s="74" t="inlineStr">
         <is>
           <t>Lender2_Percentage</t>
         </is>
@@ -4834,7 +4933,7 @@
       </c>
       <c r="AL2" s="1" t="inlineStr">
         <is>
-          <t>06-Mar-2019</t>
+          <t>25-Apr-2013</t>
         </is>
       </c>
       <c r="AM2" s="75" t="inlineStr">
@@ -4844,7 +4943,7 @@
       </c>
       <c r="AN2" s="1" t="inlineStr">
         <is>
-          <t>82627</t>
+          <t>82235</t>
         </is>
       </c>
       <c r="AO2" s="75" t="inlineStr">
@@ -4874,6 +4973,15 @@
       <c r="AU2" s="75" t="n">
         <v>20</v>
       </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="90" t="n"/>
+      <c r="D3" s="90" t="n"/>
+      <c r="AM3" s="90" t="n"/>
+      <c r="AO3" s="90" t="n"/>
+      <c r="AP3" s="90" t="n"/>
+      <c r="AQ3" s="90" t="n"/>
+      <c r="AR3" s="90" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -7103,7 +7211,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="C4" s="44" t="n"/>
       <c r="T4" s="75" t="inlineStr">
@@ -7263,16 +7370,10 @@
       <c r="AK6" s="31" t="n"/>
       <c r="AL6" s="31" t="n"/>
     </row>
-    <row r="7"/>
     <row r="8">
       <c r="R8" s="75" t="n"/>
       <c r="U8" s="30" t="n"/>
     </row>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
     <row r="14">
       <c r="C14" s="36" t="n"/>
       <c r="E14" s="36" t="n"/>
@@ -7546,7 +7647,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60000327</t>
+          <t>60000027</t>
         </is>
       </c>
       <c r="F2" s="75" t="inlineStr">
@@ -9113,7 +9214,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60000327</t>
+          <t>60000027</t>
         </is>
       </c>
       <c r="F2" s="75" t="inlineStr">

</xml_diff>